<commit_message>
Edits Reverse/M, Errors in Tratter, 6/10
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BF03F2-6C4A-1B4F-B57E-FA1295AB5C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC60A0A3-4DA9-674E-A80C-AAFE3FAC48F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="14140" yWindow="760" windowWidth="16100" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14140" yWindow="760" windowWidth="16100" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -872,8 +872,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2075,7 +2075,7 @@
         <v>76</v>
       </c>
       <c r="B72">
-        <v>197.52379999999999</v>
+        <v>201.43</v>
       </c>
       <c r="C72" t="s">
         <v>122</v>

</xml_diff>

<commit_message>
python experiments, trade friday 10/10"
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -1,39 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11003"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kostayanev/NikyClean/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC89566E-3426-3248-9B80-F18EA3A7BFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="153">
   <si>
     <t>Ticker</t>
   </si>
@@ -290,7 +271,7 @@
     <t>2025-10-03</t>
   </si>
   <si>
-    <t>2025-07-22</t>
+    <t>2025-10-23</t>
   </si>
   <si>
     <t>2025-06-24</t>
@@ -320,52 +301,58 @@
     <t>2025-06-26</t>
   </si>
   <si>
+    <t>2025-11-14</t>
+  </si>
+  <si>
+    <t>2022-08-29</t>
+  </si>
+  <si>
+    <t>2025-11-20</t>
+  </si>
+  <si>
+    <t>2025-08-28</t>
+  </si>
+  <si>
+    <t>2025-09-04</t>
+  </si>
+  <si>
+    <t>2025-08-18</t>
+  </si>
+  <si>
+    <t>2013-01-10</t>
+  </si>
+  <si>
+    <t>2025-05-02</t>
+  </si>
+  <si>
+    <t>2025-05-14</t>
+  </si>
+  <si>
+    <t>2025-03-31</t>
+  </si>
+  <si>
+    <t>2025-12-11</t>
+  </si>
+  <si>
+    <t>2024-06-14</t>
+  </si>
+  <si>
+    <t>2025-09-22</t>
+  </si>
+  <si>
+    <t>2025-04-04</t>
+  </si>
+  <si>
+    <t>2025-08-22</t>
+  </si>
+  <si>
+    <t>2024-11-18</t>
+  </si>
+  <si>
     <t>2025-08-15</t>
   </si>
   <si>
-    <t>2022-08-29</t>
-  </si>
-  <si>
-    <t>2025-08-21</t>
-  </si>
-  <si>
-    <t>2025-08-28</t>
-  </si>
-  <si>
-    <t>2025-09-04</t>
-  </si>
-  <si>
-    <t>2025-08-18</t>
-  </si>
-  <si>
-    <t>2013-01-10</t>
-  </si>
-  <si>
-    <t>2025-05-02</t>
-  </si>
-  <si>
-    <t>2025-05-14</t>
-  </si>
-  <si>
-    <t>2025-03-31</t>
-  </si>
-  <si>
-    <t>2025-09-16</t>
-  </si>
-  <si>
-    <t>2024-06-14</t>
-  </si>
-  <si>
-    <t>2025-09-22</t>
-  </si>
-  <si>
-    <t>2025-04-04</t>
-  </si>
-  <si>
-    <t>2025-08-22</t>
-  </si>
-  <si>
-    <t>2024-11-18</t>
+    <t>2025-11-24</t>
   </si>
   <si>
     <t>2025-02-20</t>
@@ -383,7 +370,7 @@
     <t>2025-09-03</t>
   </si>
   <si>
-    <t>2025-07-09</t>
+    <t>2025-10-09</t>
   </si>
   <si>
     <t>2025-03-12</t>
@@ -392,7 +379,7 @@
     <t>2025-12-02</t>
   </si>
   <si>
-    <t>2025-07-25</t>
+    <t>2025-11-07</t>
   </si>
   <si>
     <t>2015-08-21</t>
@@ -407,88 +394,73 @@
     <t>Oct 30, 2025</t>
   </si>
   <si>
-    <t>Jul 29, 2025</t>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Nov 6, 2025</t>
   </si>
   <si>
     <t>Nov 4, 2025</t>
   </si>
   <si>
-    <t>Aug 26, 2025 - Sep 1, 2025</t>
-  </si>
-  <si>
     <t>Oct 14, 2025</t>
   </si>
   <si>
     <t>Nov 12, 2025</t>
   </si>
   <si>
+    <t>Oct 29, 2025</t>
+  </si>
+  <si>
+    <t>Nov 10, 2025</t>
+  </si>
+  <si>
+    <t>Oct 28, 2025</t>
+  </si>
+  <si>
+    <t>Dec 16, 2025</t>
+  </si>
+  <si>
+    <t>Oct 21, 2025</t>
+  </si>
+  <si>
+    <t>Dec 4, 2025</t>
+  </si>
+  <si>
+    <t>Nov 25, 2025</t>
+  </si>
+  <si>
     <t>Jul 31, 2025</t>
   </si>
   <si>
-    <t>Nov 10, 2025</t>
+    <t>Oct 23, 2025</t>
+  </si>
+  <si>
+    <t>Nov 13, 2025</t>
+  </si>
+  <si>
+    <t>Oct 22, 2025</t>
+  </si>
+  <si>
+    <t>Oct 16, 2025</t>
+  </si>
+  <si>
+    <t>Sep 4, 2025</t>
+  </si>
+  <si>
+    <t>Jul 24, 2025</t>
+  </si>
+  <si>
+    <t>Oct 31, 2025</t>
+  </si>
+  <si>
+    <t>Nov 14, 2025</t>
   </si>
   <si>
     <t>Aug 6, 2025</t>
   </si>
   <si>
-    <t>Oct 28, 2025</t>
-  </si>
-  <si>
-    <t>Aug 7, 2025</t>
-  </si>
-  <si>
-    <t>Oct 21, 2025</t>
-  </si>
-  <si>
-    <t>Dec 4, 2025</t>
-  </si>
-  <si>
-    <t>Nov 25, 2025</t>
-  </si>
-  <si>
-    <t>Sep 10, 2025 - Sep 15, 2025</t>
-  </si>
-  <si>
-    <t>Nov 6, 2025</t>
-  </si>
-  <si>
-    <t>Aug 1, 2025</t>
-  </si>
-  <si>
-    <t>Oct 29, 2025</t>
-  </si>
-  <si>
-    <t>Oct 23, 2025</t>
-  </si>
-  <si>
-    <t>Oct 22, 2025</t>
-  </si>
-  <si>
-    <t>Oct 16, 2025</t>
-  </si>
-  <si>
-    <t>Aug 14, 2025</t>
-  </si>
-  <si>
-    <t>Sep 4, 2025</t>
-  </si>
-  <si>
-    <t>Jul 24, 2025</t>
-  </si>
-  <si>
-    <t>Oct 31, 2025</t>
-  </si>
-  <si>
-    <t>Aug 12, 2025</t>
-  </si>
-  <si>
-    <t>Jul 17, 2025</t>
-  </si>
-  <si>
     <t>Nov 3, 2025</t>
-  </si>
-  <si>
-    <t>Jul 22, 2025</t>
   </si>
   <si>
     <t>USD</t>
@@ -506,8 +478,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00%"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,34 +534,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -624,7 +590,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -658,7 +624,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -693,10 +658,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -869,20 +833,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -902,27 +863,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2">
-        <v>235.52553</v>
+        <v>248.17128</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E2" s="1">
-        <v>4.3E-3</v>
+        <v>0.0042</v>
       </c>
       <c r="F2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -933,171 +894,171 @@
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>1.2999999E-2</v>
+        <v>0.0127</v>
       </c>
       <c r="F3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4">
-        <v>95.060005000000004</v>
+        <v>96.66</v>
       </c>
       <c r="F4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5">
-        <v>263.18033000000003</v>
+        <v>266.5645</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.5333300000000001</v>
+        <v>1.53333</v>
+      </c>
+      <c r="D6" t="s">
+        <v>126</v>
       </c>
       <c r="F6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7">
-        <v>758</v>
+        <v>873.90326</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
       </c>
       <c r="E7" s="1">
-        <v>9.7999999999999997E-3</v>
+        <v>0.008</v>
       </c>
       <c r="F7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8">
-        <v>87.27</v>
+        <v>89.77</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="E8" s="1">
-        <v>1.9199998999999999E-2</v>
+        <v>0.0185</v>
       </c>
       <c r="F8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
-        <v>2.3158300000000001</v>
+        <v>2.4325</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>126</v>
-      </c>
       <c r="F10" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11">
-        <v>101.54761999999999</v>
+        <v>110.64286</v>
       </c>
       <c r="C11" t="s">
         <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1">
-        <v>2.52E-2</v>
+        <v>0.0256</v>
       </c>
       <c r="F11" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12">
-        <v>75.814760000000007</v>
+        <v>76.29095</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E12" s="1">
-        <v>2.4500001E-2</v>
+        <v>0.0241</v>
       </c>
       <c r="F12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13">
-        <v>82.072500000000005</v>
+        <v>83.79167</v>
       </c>
       <c r="C13" t="s">
         <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E13" s="1">
-        <v>3.61E-2</v>
+        <v>0.0341</v>
       </c>
       <c r="F13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1105,64 +1066,61 @@
         <v>3.25</v>
       </c>
       <c r="D14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15">
-        <v>132.22594000000001</v>
+        <v>133.96896</v>
       </c>
       <c r="C15" t="s">
         <v>86</v>
       </c>
-      <c r="D15" t="s">
-        <v>131</v>
-      </c>
       <c r="E15" s="1">
-        <v>8.5000000000000006E-3</v>
+        <v>0.0092</v>
       </c>
       <c r="F15" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16">
-        <v>35.563890000000001</v>
+        <v>35.35278</v>
       </c>
       <c r="C16" t="s">
         <v>87</v>
       </c>
       <c r="E16" s="1">
-        <v>9.7000000000000003E-3</v>
+        <v>0.0091</v>
       </c>
       <c r="F16" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17">
-        <v>153.5</v>
+        <v>151.5</v>
       </c>
       <c r="D17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1173,30 +1131,30 @@
         <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19">
-        <v>16.88824</v>
+        <v>16.88235</v>
       </c>
       <c r="C19" t="s">
         <v>89</v>
       </c>
       <c r="E19" s="1">
-        <v>3.6199997999999997E-2</v>
+        <v>0.0342</v>
       </c>
       <c r="F19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1204,260 +1162,257 @@
         <v>90</v>
       </c>
       <c r="D20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F20" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21">
-        <v>57.2</v>
+        <v>63.8</v>
       </c>
       <c r="C21" t="s">
         <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E21" s="1">
-        <v>1.0299999000000001E-2</v>
+        <v>0.0108</v>
       </c>
       <c r="F21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22">
-        <v>24.984120000000001</v>
+        <v>26.04056</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E22" s="1">
-        <v>2.2100000000000002E-2</v>
+        <v>0.021300001</v>
       </c>
       <c r="F22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23">
-        <v>27.968</v>
+        <v>28.16375</v>
       </c>
       <c r="C23" t="s">
         <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E23" s="1">
-        <v>3.95E-2</v>
+        <v>0.045300003</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24">
-        <v>435.83789999999999</v>
+        <v>438.45612</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
       </c>
       <c r="E24" s="1">
-        <v>1.9599999999999999E-2</v>
+        <v>0.0188</v>
       </c>
       <c r="F24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25">
-        <v>75.727270000000004</v>
+        <v>76.27273</v>
       </c>
       <c r="C25" t="s">
         <v>95</v>
       </c>
       <c r="D25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" s="1">
-        <v>2.07E-2</v>
+        <v>0.0207</v>
       </c>
       <c r="F25" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26">
         <v>15</v>
       </c>
-      <c r="D26" t="s">
-        <v>138</v>
-      </c>
       <c r="F26" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27">
-        <v>5.06182</v>
+        <v>5.24364</v>
       </c>
       <c r="C27" t="s">
         <v>96</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="F27" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28">
-        <v>44.25</v>
+        <v>44.3</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29">
-        <v>613.89160000000004</v>
+        <v>620.7369</v>
       </c>
       <c r="C29" t="s">
         <v>97</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E29" s="1">
-        <v>6.7000002999999999E-3</v>
+        <v>0.0070999996</v>
       </c>
       <c r="F29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30">
-        <v>82.294120000000007</v>
+        <v>84.72221999999999</v>
       </c>
       <c r="C30" t="s">
         <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E30" s="1">
-        <v>3.2000000000000001E-2</v>
+        <v>0.0272</v>
       </c>
       <c r="F30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31">
-        <v>73.224739999999997</v>
+        <v>91.20950000000001</v>
       </c>
       <c r="C31" t="s">
         <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E31" s="1">
-        <v>1.3099998999999999E-2</v>
+        <v>0.0117</v>
       </c>
       <c r="F31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="B32">
-        <v>1350.316</v>
+        <v>1358.6105</v>
       </c>
       <c r="D32" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>37</v>
       </c>
       <c r="B33">
-        <v>31.501259999999998</v>
+        <v>31.50108</v>
       </c>
       <c r="F33" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>38</v>
       </c>
       <c r="B34">
-        <v>37.375</v>
+        <v>44.5</v>
       </c>
       <c r="C34" t="s">
         <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E34" s="1">
-        <v>1.3899999999999999E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="F34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1465,24 +1420,24 @@
         <v>12.1</v>
       </c>
       <c r="F35" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>40</v>
       </c>
       <c r="B36">
-        <v>6.6333299999999999</v>
+        <v>6.63333</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F36" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -1490,58 +1445,58 @@
         <v>101</v>
       </c>
       <c r="F37" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>42</v>
       </c>
       <c r="B38">
-        <v>38.333329999999997</v>
+        <v>38.33333</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F38" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>43</v>
       </c>
       <c r="B39">
-        <v>43.26</v>
+        <v>43.98235</v>
       </c>
       <c r="C39" t="s">
         <v>102</v>
       </c>
       <c r="E39" s="1">
-        <v>3.1400003000000003E-2</v>
+        <v>0.0272</v>
       </c>
       <c r="F39" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>44</v>
       </c>
       <c r="B40">
-        <v>291.91037</v>
+        <v>287.6027</v>
       </c>
       <c r="C40" t="s">
         <v>103</v>
       </c>
       <c r="E40" s="1">
-        <v>1.0299999000000001E-2</v>
+        <v>0.010199999</v>
       </c>
       <c r="F40" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -1549,13 +1504,13 @@
         <v>104</v>
       </c>
       <c r="E41" s="1">
-        <v>2.47E-2</v>
+        <v>0.0232</v>
       </c>
       <c r="F41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -1563,89 +1518,89 @@
         <v>13.33333</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F42" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>47</v>
       </c>
       <c r="B43">
-        <v>310.53410000000002</v>
+        <v>360.62946</v>
       </c>
       <c r="D43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F43" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>48</v>
       </c>
       <c r="B44">
-        <v>274.15667999999999</v>
+        <v>307.64688</v>
       </c>
       <c r="C44" t="s">
         <v>105</v>
       </c>
       <c r="D44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E44" s="1">
-        <v>1.37E-2</v>
+        <v>0.0119</v>
       </c>
       <c r="F44" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>50</v>
       </c>
       <c r="B46">
-        <v>8.2502700000000004</v>
+        <v>7.475</v>
       </c>
       <c r="C46" t="s">
         <v>106</v>
       </c>
       <c r="D46" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="F46" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>51</v>
       </c>
       <c r="B47">
-        <v>355.06</v>
+        <v>370.3649</v>
       </c>
       <c r="C47" t="s">
         <v>107</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E47" s="1">
-        <v>6.9999998000000001E-3</v>
+        <v>0.0073</v>
       </c>
       <c r="F47" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -1656,53 +1611,53 @@
         <v>108</v>
       </c>
       <c r="E48" s="1">
-        <v>2.7099999999999999E-2</v>
+        <v>0.028800001</v>
       </c>
       <c r="F48" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49">
-        <v>63.325000000000003</v>
+        <v>61.1</v>
       </c>
       <c r="C49" t="s">
         <v>108</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E49" s="1">
-        <v>4.8800003000000002E-2</v>
+        <v>0.0493</v>
       </c>
       <c r="F49" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>54</v>
       </c>
       <c r="B50">
-        <v>11.428570000000001</v>
+        <v>11.42857</v>
       </c>
       <c r="C50" t="s">
         <v>109</v>
       </c>
       <c r="D50" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E50" s="1">
-        <v>4.5700002000000003E-2</v>
+        <v>0.0493</v>
       </c>
       <c r="F50" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1713,44 +1668,44 @@
         <v>110</v>
       </c>
       <c r="E51" s="1">
-        <v>8.3500005000000002E-2</v>
+        <v>0.083500005</v>
       </c>
       <c r="F51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>56</v>
       </c>
       <c r="B52">
-        <v>124.79167</v>
+        <v>124.4512</v>
       </c>
       <c r="C52" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D52" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E52" s="1">
-        <v>3.6299999999999999E-2</v>
+        <v>0.0358</v>
       </c>
       <c r="F52" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>57</v>
       </c>
       <c r="B53">
-        <v>11</v>
+        <v>11.4</v>
       </c>
       <c r="F53" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -1758,178 +1713,178 @@
         <v>2.4</v>
       </c>
       <c r="D54" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>59</v>
       </c>
       <c r="B55">
-        <v>15.5</v>
-      </c>
-      <c r="C55" s="3">
-        <v>45985</v>
+        <v>15.58636</v>
+      </c>
+      <c r="C55" t="s">
+        <v>112</v>
       </c>
       <c r="E55" s="1">
-        <v>7.1100003999999994E-2</v>
+        <v>0.06950000000000001</v>
       </c>
       <c r="F55" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>60</v>
       </c>
       <c r="B56">
-        <v>658.68399999999997</v>
+        <v>643.684</v>
       </c>
       <c r="C56" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E56" s="1">
-        <v>2.5799999000000001E-2</v>
+        <v>0.026099999</v>
       </c>
       <c r="F56" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>61</v>
       </c>
       <c r="B57">
-        <v>10.8</v>
+        <v>11.475</v>
       </c>
       <c r="C57" t="s">
         <v>79</v>
       </c>
       <c r="D57" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E57" s="1">
-        <v>5.11E-2</v>
+        <v>0.052600004</v>
       </c>
       <c r="F57" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>62</v>
       </c>
       <c r="B58">
-        <v>61.800559999999997</v>
+        <v>63.15722</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D58" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E58" s="1">
-        <v>3.2099999999999997E-2</v>
+        <v>0.031600002</v>
       </c>
       <c r="F58" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>63</v>
       </c>
       <c r="B59">
-        <v>204.5</v>
+        <v>203.375</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F59" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>64</v>
       </c>
       <c r="B60">
-        <v>710.57899999999995</v>
+        <v>764.6842</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E60" s="1">
-        <v>2.1700000000000001E-2</v>
+        <v>0.0209</v>
       </c>
       <c r="F60" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>65</v>
       </c>
       <c r="B61">
-        <v>2.6666699999999999</v>
+        <v>2.66667</v>
       </c>
       <c r="D61" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F61" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>66</v>
       </c>
       <c r="B62">
-        <v>32.06</v>
+        <v>33.06</v>
       </c>
       <c r="C62" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E62" s="1">
-        <v>2.29E-2</v>
+        <v>0.023</v>
       </c>
       <c r="F62" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>67</v>
       </c>
       <c r="B63">
-        <v>644.55150000000003</v>
+        <v>648.4303</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D63" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E63" s="1">
-        <v>5.1999999999999998E-3</v>
+        <v>0.0055</v>
       </c>
       <c r="F63" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -1937,168 +1892,168 @@
         <v>12.5</v>
       </c>
       <c r="D64" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="F64" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>69</v>
       </c>
       <c r="B65">
-        <v>118.545</v>
+        <v>122.054</v>
       </c>
       <c r="C65" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D65" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="E65" s="1">
-        <v>3.0800000000000001E-2</v>
+        <v>0.0307</v>
       </c>
       <c r="F65" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>70</v>
       </c>
       <c r="B66">
-        <v>14.994440000000001</v>
+        <v>15.28889</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E66" s="1">
-        <v>5.5E-2</v>
+        <v>0.0552</v>
       </c>
       <c r="F66" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>71</v>
       </c>
       <c r="B67">
-        <v>50.78</v>
+        <v>51.54545</v>
       </c>
       <c r="C67" t="s">
         <v>93</v>
       </c>
       <c r="D67" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="E67" s="1">
-        <v>2.0899999999999998E-2</v>
+        <v>0.0228</v>
       </c>
       <c r="F67" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>72</v>
       </c>
       <c r="B68">
-        <v>28.857140000000001</v>
+        <v>28.80864</v>
       </c>
       <c r="C68" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D68" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="E68" s="1">
-        <v>6.9099999999999995E-2</v>
+        <v>0.0694</v>
       </c>
       <c r="F68" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>73</v>
       </c>
       <c r="B69">
-        <v>3.8769200000000001</v>
+        <v>3.87692</v>
       </c>
       <c r="C69" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D69" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F69" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>74</v>
       </c>
       <c r="B70">
-        <v>42.625</v>
+        <v>42.25</v>
       </c>
       <c r="C70" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D70" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E70" s="1">
-        <v>1.04E-2</v>
+        <v>0.009900000000000001</v>
       </c>
       <c r="F70" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>75</v>
       </c>
       <c r="B71">
-        <v>85.644440000000003</v>
+        <v>88.00556</v>
       </c>
       <c r="D71" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F71" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>76</v>
       </c>
       <c r="B72">
-        <v>201.43</v>
+        <v>204.90475</v>
       </c>
       <c r="C72" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D72" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="F72" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>78</v>
       </c>
       <c r="F74" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trades_extended_gui.py, README.md, TRADES_User_Guide.pdf, TRADES.xlsx branch testlog
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="146">
   <si>
     <t>Ticker</t>
   </si>
@@ -256,7 +256,7 @@
     <t>2025-11-10</t>
   </si>
   <si>
-    <t>2025-08-26</t>
+    <t>2025-11-24</t>
   </si>
   <si>
     <t>2025-10-28</t>
@@ -271,13 +271,13 @@
     <t>2025-11-03</t>
   </si>
   <si>
-    <t>2025-10-03</t>
+    <t>2026-01-02</t>
   </si>
   <si>
     <t>2025-10-23</t>
   </si>
   <si>
-    <t>2025-06-24</t>
+    <t>2025-12-15</t>
   </si>
   <si>
     <t>2025-05-26</t>
@@ -301,7 +301,7 @@
     <t>2025-09-10</t>
   </si>
   <si>
-    <t>2025-06-26</t>
+    <t>2025-11-27</t>
   </si>
   <si>
     <t>2025-11-14</t>
@@ -319,9 +319,6 @@
     <t>2025-11-26</t>
   </si>
   <si>
-    <t>2025-08-18</t>
-  </si>
-  <si>
     <t>2013-01-10</t>
   </si>
   <si>
@@ -343,12 +340,6 @@
     <t>2025-04-04</t>
   </si>
   <si>
-    <t>2025-08-22</t>
-  </si>
-  <si>
-    <t>2025-11-24</t>
-  </si>
-  <si>
     <t>2025-02-20</t>
   </si>
   <si>
@@ -364,7 +355,7 @@
     <t>2025-12-02</t>
   </si>
   <si>
-    <t>2025-09-03</t>
+    <t>2025-12-26</t>
   </si>
   <si>
     <t>2025-10-09</t>
@@ -373,6 +364,9 @@
     <t>2025-03-12</t>
   </si>
   <si>
+    <t>2025-12-10</t>
+  </si>
+  <si>
     <t>2015-08-21</t>
   </si>
   <si>
@@ -400,46 +394,49 @@
     <t>Jan 14, 2026</t>
   </si>
   <si>
+    <t>Feb 11, 2026</t>
+  </si>
+  <si>
+    <t>Oct 29, 2025</t>
+  </si>
+  <si>
+    <t>Nov 4, 2025</t>
+  </si>
+  <si>
+    <t>Jan 27, 2026</t>
+  </si>
+  <si>
+    <t>Dec 4, 2025</t>
+  </si>
+  <si>
+    <t>Nov 25, 2025</t>
+  </si>
+  <si>
+    <t>Jan 28, 2026</t>
+  </si>
+  <si>
+    <t>Jan 23, 2026</t>
+  </si>
+  <si>
+    <t>Oct 23, 2025</t>
+  </si>
+  <si>
+    <t>Jan 20, 2026</t>
+  </si>
+  <si>
     <t>Nov 12, 2025</t>
   </si>
   <si>
-    <t>Oct 29, 2025</t>
-  </si>
-  <si>
-    <t>Nov 4, 2025</t>
-  </si>
-  <si>
-    <t>Oct 21, 2025</t>
-  </si>
-  <si>
-    <t>Dec 4, 2025</t>
-  </si>
-  <si>
-    <t>Nov 25, 2025</t>
-  </si>
-  <si>
-    <t>Jan 28, 2026</t>
+    <t>Jan 15, 2026</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Jan 30, 2026</t>
   </si>
   <si>
     <t>Oct 28, 2025</t>
-  </si>
-  <si>
-    <t>Oct 23, 2025</t>
-  </si>
-  <si>
-    <t>Jan 20, 2026</t>
-  </si>
-  <si>
-    <t>Jan 15, 2026</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Jan 30, 2026</t>
-  </si>
-  <si>
-    <t>Oct 22, 2025</t>
   </si>
   <si>
     <t>Nov 10, 2025</t>
@@ -850,19 +847,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>276.43097</v>
+        <v>281.74805</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="1">
         <v>0.0038</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -870,16 +867,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>20.66667</v>
+        <v>19.75</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0117</v>
+        <v>0.0166</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -890,7 +887,7 @@
         <v>96.66</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -898,13 +895,13 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>288.4241</v>
+        <v>294.9145</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -912,10 +909,10 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.53333</v>
+        <v>1.56667</v>
       </c>
       <c r="F6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -923,16 +920,16 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>941.90326</v>
+        <v>952.70966</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0069999998</v>
+        <v>0.0077</v>
       </c>
       <c r="F7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -940,19 +937,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>392.38165</v>
+        <v>399.9678</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0064</v>
+        <v>0.0069</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -960,19 +957,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>93.25273</v>
+        <v>93.15273000000001</v>
       </c>
       <c r="C9" t="s">
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" s="1">
-        <v>0.019</v>
+        <v>0.0172</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -980,13 +977,13 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>2.75</v>
+        <v>2.9875</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -994,7 +991,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1002,19 +999,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>113.7619</v>
+        <v>114.33333</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" s="1">
-        <v>0.023699999</v>
+        <v>0.024300002</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1022,19 +1019,19 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>76.29095</v>
+        <v>84.81476000000001</v>
       </c>
       <c r="C13" t="s">
         <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0224</v>
+        <v>0.0216</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1042,19 +1039,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>90.48</v>
+        <v>91.48</v>
       </c>
       <c r="C14" t="s">
         <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E14" s="1">
-        <v>0.034</v>
+        <v>0.0341</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1062,13 +1059,13 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>3.25</v>
+        <v>3.625</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1076,19 +1073,19 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>134.0724</v>
+        <v>132.50357</v>
       </c>
       <c r="C16" t="s">
         <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0089</v>
+        <v>0.014400001</v>
       </c>
       <c r="F16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1102,10 +1099,10 @@
         <v>88</v>
       </c>
       <c r="E17" s="1">
-        <v>0.0106</v>
+        <v>0.0111</v>
       </c>
       <c r="F17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1113,13 +1110,13 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>147.125</v>
+        <v>144.5</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1133,10 +1130,10 @@
         <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1144,16 +1141,16 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>16.91959</v>
+        <v>16.93418</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0341</v>
+        <v>0.0355</v>
       </c>
       <c r="F20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1164,7 +1161,7 @@
         <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1172,19 +1169,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>73.15385000000001</v>
+        <v>74.15385000000001</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E22" s="1">
-        <v>0.008699999999999999</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1192,19 +1189,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>26.51211</v>
+        <v>26.5</v>
       </c>
       <c r="C23" t="s">
         <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E23" s="1">
-        <v>0.021300001</v>
+        <v>0.0253</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1212,19 +1209,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>28.2825</v>
+        <v>27.7375</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0418</v>
+        <v>0.048299998</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1232,16 +1229,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>464.0942</v>
+        <v>464.9328</v>
       </c>
       <c r="C25" t="s">
         <v>95</v>
       </c>
       <c r="E25" s="1">
-        <v>0.0183</v>
+        <v>0.0247</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1255,13 +1252,13 @@
         <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E26" s="1">
-        <v>0.022</v>
+        <v>0.0212</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1272,7 +1269,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1280,16 +1277,16 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>5.958</v>
+        <v>6.858</v>
       </c>
       <c r="C28" t="s">
         <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1297,13 +1294,13 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>40.3</v>
+        <v>37.31579</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1311,19 +1308,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>626.2265599999999</v>
+        <v>625.4096</v>
       </c>
       <c r="C30" t="s">
         <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E30" s="1">
-        <v>0.0069999998</v>
+        <v>0.0077</v>
       </c>
       <c r="F30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1337,13 +1334,13 @@
         <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E31" s="1">
-        <v>0.0278</v>
+        <v>0.0271</v>
       </c>
       <c r="F31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1351,19 +1348,19 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>102.735</v>
+        <v>103.57</v>
       </c>
       <c r="C32" t="s">
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0124</v>
+        <v>0.012</v>
       </c>
       <c r="F32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1371,13 +1368,13 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>1347.3231</v>
+        <v>134.65277</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1385,10 +1382,10 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>31.50108</v>
+        <v>19.25054</v>
       </c>
       <c r="F34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1396,19 +1393,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>46.875</v>
+        <v>47.125</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E35" s="1">
-        <v>0.0136</v>
+        <v>0.0152</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1419,7 +1416,7 @@
         <v>12.1</v>
       </c>
       <c r="F36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1427,13 +1424,13 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>6.63333</v>
+        <v>6.6</v>
       </c>
       <c r="D37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1441,10 +1438,10 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1452,13 +1449,13 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>38.33333</v>
+        <v>49.6</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1466,16 +1463,16 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>44.74706</v>
+        <v>47.23529</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E40" s="1">
-        <v>0.025799999</v>
+        <v>0.025</v>
       </c>
       <c r="F40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1483,16 +1480,16 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>288.6668</v>
+        <v>287.58334</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="1">
-        <v>0.0105</v>
+        <v>0.0115</v>
       </c>
       <c r="F41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1500,13 +1497,16 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
       </c>
       <c r="E42" s="1">
-        <v>0.024500001</v>
+        <v>0.0256</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1514,13 +1514,13 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>13.33333</v>
+        <v>13.16667</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1528,13 +1528,13 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>391.31805</v>
+        <v>392.9278</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1542,19 +1542,19 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>335.39688</v>
+        <v>341.90668</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0111</v>
+        <v>0.0124</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1567,16 +1567,16 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>7.42222</v>
+        <v>7.2</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1584,19 +1584,19 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>392.38165</v>
+        <v>399.9678</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E48" s="1">
-        <v>0.0064</v>
+        <v>0.0069</v>
       </c>
       <c r="F48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1607,13 +1607,13 @@
         <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E49" s="1">
-        <v>0.0291</v>
+        <v>0.028199999</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1621,19 +1621,19 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>61.5</v>
+        <v>62.66667</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E50" s="1">
-        <v>0.049200002</v>
+        <v>0.0504</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1641,19 +1641,19 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>12.125</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" s="1">
-        <v>0.0463</v>
+        <v>0.0458</v>
       </c>
       <c r="F51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1666,19 +1666,19 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>126.88</v>
+        <v>128.72</v>
       </c>
       <c r="C53" t="s">
         <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E53" s="1">
-        <v>0.0346</v>
+        <v>0.0352</v>
       </c>
       <c r="F53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1689,7 +1689,7 @@
         <v>11.4</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1700,10 +1700,10 @@
         <v>2.4</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1711,16 +1711,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>16.12273</v>
+        <v>16.30909</v>
       </c>
       <c r="C56" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="E56" s="1">
-        <v>0.06519999999999999</v>
+        <v>0.0646</v>
       </c>
       <c r="F56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1731,13 +1731,13 @@
         <v>626.25</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E57" s="1">
-        <v>0.025</v>
+        <v>0.026099999</v>
       </c>
       <c r="F57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1745,19 +1745,19 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>12.265</v>
+        <v>12.415</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E58" s="1">
-        <v>0.045700002</v>
+        <v>0.0468</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1765,19 +1765,19 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>64.68611</v>
+        <v>65.35278</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E59" s="1">
-        <v>0.031</v>
+        <v>0.0301</v>
       </c>
       <c r="F59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1785,16 +1785,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>207.4706</v>
+        <v>206</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1802,19 +1802,19 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>801.8421</v>
+        <v>802.5263</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E61" s="1">
-        <v>0.020299999</v>
+        <v>0.0207</v>
       </c>
       <c r="F61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1822,13 +1822,13 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>2.5</v>
+        <v>14.99999</v>
       </c>
       <c r="D62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1836,19 +1836,19 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>34.07368</v>
+        <v>34.23158</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="E63" s="1">
-        <v>0.0238</v>
+        <v>0.022</v>
       </c>
       <c r="F63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1856,19 +1856,19 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>655.2057</v>
+        <v>656.50555</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E64" s="1">
-        <v>0.0055</v>
+        <v>0.0056</v>
       </c>
       <c r="F64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1876,13 +1876,13 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>12.6125</v>
+        <v>12.66667</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="F65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1890,19 +1890,19 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>127.454</v>
+        <v>131.28</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E66" s="1">
-        <v>0.0323</v>
+        <v>0.031400003</v>
       </c>
       <c r="F66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1910,16 +1910,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>15.32222</v>
+        <v>15.47647</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E67" s="1">
-        <v>0.0542</v>
+        <v>0.0538</v>
       </c>
       <c r="F67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1927,19 +1927,19 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>49.91304</v>
+        <v>50.20833</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E68" s="1">
-        <v>0.0233</v>
+        <v>0.0232</v>
       </c>
       <c r="F68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1947,19 +1947,19 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>28.7519</v>
+        <v>29.03958</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E69" s="1">
-        <v>0.0698</v>
+        <v>0.0687</v>
       </c>
       <c r="F69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1967,16 +1967,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>3.95385</v>
+        <v>4.16538</v>
       </c>
       <c r="C70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1984,19 +1984,19 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>41.41542</v>
+        <v>42.04348</v>
       </c>
       <c r="C71" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D71" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E71" s="1">
-        <v>0.0101</v>
+        <v>0.0095</v>
       </c>
       <c r="F71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2004,13 +2004,13 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>88.50526000000001</v>
+        <v>84.00526000000001</v>
       </c>
       <c r="D72" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2018,16 +2018,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>229.61905</v>
+        <v>233.42857</v>
       </c>
       <c r="C73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D73" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2040,7 +2040,7 @@
         <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
25/11, RIGL48.28, MEDY Yahoo update, Entries SCAN
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="146">
   <si>
     <t>Ticker</t>
   </si>
@@ -256,7 +256,7 @@
     <t>2025-11-10</t>
   </si>
   <si>
-    <t>2025-08-26</t>
+    <t>2025-11-24</t>
   </si>
   <si>
     <t>2025-10-28</t>
@@ -271,13 +271,13 @@
     <t>2025-11-03</t>
   </si>
   <si>
-    <t>2025-10-03</t>
+    <t>2026-01-02</t>
   </si>
   <si>
     <t>2025-10-23</t>
   </si>
   <si>
-    <t>2025-06-24</t>
+    <t>2025-12-15</t>
   </si>
   <si>
     <t>2025-05-26</t>
@@ -301,7 +301,7 @@
     <t>2025-09-10</t>
   </si>
   <si>
-    <t>2025-06-26</t>
+    <t>2025-11-27</t>
   </si>
   <si>
     <t>2025-11-14</t>
@@ -319,9 +319,6 @@
     <t>2025-11-26</t>
   </si>
   <si>
-    <t>2025-08-18</t>
-  </si>
-  <si>
     <t>2013-01-10</t>
   </si>
   <si>
@@ -343,12 +340,6 @@
     <t>2025-04-04</t>
   </si>
   <si>
-    <t>2025-08-22</t>
-  </si>
-  <si>
-    <t>2025-11-24</t>
-  </si>
-  <si>
     <t>2025-02-20</t>
   </si>
   <si>
@@ -364,7 +355,7 @@
     <t>2025-12-02</t>
   </si>
   <si>
-    <t>2025-09-03</t>
+    <t>2025-12-26</t>
   </si>
   <si>
     <t>2025-10-09</t>
@@ -373,6 +364,9 @@
     <t>2025-03-12</t>
   </si>
   <si>
+    <t>2025-12-10</t>
+  </si>
+  <si>
     <t>2015-08-21</t>
   </si>
   <si>
@@ -400,46 +394,49 @@
     <t>Jan 14, 2026</t>
   </si>
   <si>
+    <t>Feb 11, 2026</t>
+  </si>
+  <si>
+    <t>Oct 29, 2025</t>
+  </si>
+  <si>
+    <t>Nov 4, 2025</t>
+  </si>
+  <si>
+    <t>Jan 27, 2026</t>
+  </si>
+  <si>
+    <t>Dec 4, 2025</t>
+  </si>
+  <si>
+    <t>Nov 25, 2025</t>
+  </si>
+  <si>
+    <t>Jan 28, 2026</t>
+  </si>
+  <si>
+    <t>Jan 23, 2026</t>
+  </si>
+  <si>
+    <t>Oct 23, 2025</t>
+  </si>
+  <si>
+    <t>Jan 20, 2026</t>
+  </si>
+  <si>
     <t>Nov 12, 2025</t>
   </si>
   <si>
-    <t>Oct 29, 2025</t>
-  </si>
-  <si>
-    <t>Nov 4, 2025</t>
-  </si>
-  <si>
-    <t>Oct 21, 2025</t>
-  </si>
-  <si>
-    <t>Dec 4, 2025</t>
-  </si>
-  <si>
-    <t>Nov 25, 2025</t>
-  </si>
-  <si>
-    <t>Jan 28, 2026</t>
+    <t>Jan 15, 2026</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Jan 30, 2026</t>
   </si>
   <si>
     <t>Oct 28, 2025</t>
-  </si>
-  <si>
-    <t>Oct 23, 2025</t>
-  </si>
-  <si>
-    <t>Jan 20, 2026</t>
-  </si>
-  <si>
-    <t>Jan 15, 2026</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Jan 30, 2026</t>
-  </si>
-  <si>
-    <t>Oct 22, 2025</t>
   </si>
   <si>
     <t>Nov 10, 2025</t>
@@ -850,19 +847,19 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>276.43097</v>
+        <v>281.74805</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E2" s="1">
         <v>0.0038</v>
       </c>
       <c r="F2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -870,16 +867,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>20.66667</v>
+        <v>19.75</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0117</v>
+        <v>0.0164</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -887,10 +884,10 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>96.66</v>
+        <v>95.26000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -898,13 +895,13 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>288.4241</v>
+        <v>294.9145</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -912,10 +909,10 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>1.53333</v>
+        <v>1.56667</v>
       </c>
       <c r="F6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -923,16 +920,16 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>941.90326</v>
+        <v>953.6774</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0069999998</v>
+        <v>0.0075</v>
       </c>
       <c r="F7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -940,19 +937,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>392.38165</v>
+        <v>399.9678</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0064</v>
+        <v>0.0062</v>
       </c>
       <c r="F8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -960,19 +957,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>93.25273</v>
+        <v>94.68273000000001</v>
       </c>
       <c r="C9" t="s">
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" s="1">
-        <v>0.019</v>
+        <v>0.0171</v>
       </c>
       <c r="F9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -980,13 +977,13 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>2.75</v>
+        <v>2.9875</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -994,7 +991,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1002,19 +999,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>113.7619</v>
+        <v>114.33333</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E12" s="1">
-        <v>0.023699999</v>
+        <v>0.0241</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1022,19 +1019,19 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>76.29095</v>
+        <v>84.81476000000001</v>
       </c>
       <c r="C13" t="s">
         <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0224</v>
+        <v>0.0215</v>
       </c>
       <c r="F13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1042,19 +1039,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>90.48</v>
+        <v>91.48</v>
       </c>
       <c r="C14" t="s">
         <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E14" s="1">
-        <v>0.034</v>
+        <v>0.0341</v>
       </c>
       <c r="F14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1062,13 +1059,13 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>3.25</v>
+        <v>3.625</v>
       </c>
       <c r="D15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1076,19 +1073,19 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>134.0724</v>
+        <v>132.50357</v>
       </c>
       <c r="C16" t="s">
         <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0089</v>
+        <v>0.0147</v>
       </c>
       <c r="F16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1102,10 +1099,10 @@
         <v>88</v>
       </c>
       <c r="E17" s="1">
-        <v>0.0106</v>
+        <v>0.0109</v>
       </c>
       <c r="F17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1113,13 +1110,13 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>147.125</v>
+        <v>144.5</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1133,10 +1130,10 @@
         <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1144,16 +1141,16 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>16.91959</v>
+        <v>16.93418</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0341</v>
+        <v>0.0359</v>
       </c>
       <c r="F20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1164,7 +1161,7 @@
         <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1172,19 +1169,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>73.15385000000001</v>
+        <v>74.15385000000001</v>
       </c>
       <c r="C22" t="s">
         <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E22" s="1">
-        <v>0.008699999999999999</v>
+        <v>0.008500000000000001</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1192,19 +1189,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>26.51211</v>
+        <v>26.5</v>
       </c>
       <c r="C23" t="s">
         <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E23" s="1">
-        <v>0.021300001</v>
+        <v>0.0247</v>
       </c>
       <c r="F23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1212,19 +1209,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>28.2825</v>
+        <v>27.7375</v>
       </c>
       <c r="C24" t="s">
         <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0418</v>
+        <v>0.0475</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1232,16 +1229,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>464.0942</v>
+        <v>463.54266</v>
       </c>
       <c r="C25" t="s">
         <v>95</v>
       </c>
       <c r="E25" s="1">
-        <v>0.0183</v>
+        <v>0.024</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1255,13 +1252,13 @@
         <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E26" s="1">
-        <v>0.022</v>
+        <v>0.0218</v>
       </c>
       <c r="F26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1272,7 +1269,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1280,16 +1277,16 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>5.958</v>
+        <v>7.233</v>
       </c>
       <c r="C28" t="s">
         <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1297,13 +1294,13 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>40.3</v>
+        <v>37.31579</v>
       </c>
       <c r="D29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1311,19 +1308,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>626.2265599999999</v>
+        <v>625.4096</v>
       </c>
       <c r="C30" t="s">
         <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E30" s="1">
-        <v>0.0069999998</v>
+        <v>0.0077</v>
       </c>
       <c r="F30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1337,13 +1334,13 @@
         <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E31" s="1">
-        <v>0.0278</v>
+        <v>0.0269</v>
       </c>
       <c r="F31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1351,19 +1348,19 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>102.735</v>
+        <v>103.57</v>
       </c>
       <c r="C32" t="s">
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0124</v>
+        <v>0.0116</v>
       </c>
       <c r="F32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1371,13 +1368,13 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>1347.3231</v>
+        <v>134.65277</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F33" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1385,10 +1382,10 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>31.50108</v>
+        <v>19.25054</v>
       </c>
       <c r="F34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1396,19 +1393,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>46.875</v>
+        <v>47.125</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E35" s="1">
-        <v>0.0136</v>
+        <v>0.014400001</v>
       </c>
       <c r="F35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1419,7 +1416,7 @@
         <v>12.1</v>
       </c>
       <c r="F36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1427,13 +1424,13 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>6.63333</v>
+        <v>6.6</v>
       </c>
       <c r="D37" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1441,10 +1438,10 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1452,13 +1449,13 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>38.33333</v>
+        <v>49.6</v>
       </c>
       <c r="D39" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1466,16 +1463,16 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>44.74706</v>
+        <v>47.23529</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E40" s="1">
-        <v>0.025799999</v>
+        <v>0.025</v>
       </c>
       <c r="F40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1483,16 +1480,16 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>288.6668</v>
+        <v>287.58334</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E41" s="1">
-        <v>0.0105</v>
+        <v>0.0113</v>
       </c>
       <c r="F41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1500,13 +1497,16 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>132</v>
       </c>
       <c r="E42" s="1">
-        <v>0.024500001</v>
+        <v>0.0253</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1514,13 +1514,13 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>13.33333</v>
+        <v>13.16667</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1528,13 +1528,13 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>391.31805</v>
+        <v>392.9278</v>
       </c>
       <c r="D44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1542,19 +1542,19 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>335.39688</v>
+        <v>341.90668</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0111</v>
+        <v>0.012</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1567,16 +1567,16 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>7.42222</v>
+        <v>7.2</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1584,19 +1584,19 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>392.38165</v>
+        <v>399.9678</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E48" s="1">
-        <v>0.0064</v>
+        <v>0.0062</v>
       </c>
       <c r="F48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1607,13 +1607,13 @@
         <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E49" s="1">
-        <v>0.0291</v>
+        <v>0.0278</v>
       </c>
       <c r="F49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1621,19 +1621,19 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>61.5</v>
+        <v>62.66667</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E50" s="1">
-        <v>0.049200002</v>
+        <v>0.050300002</v>
       </c>
       <c r="F50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1641,19 +1641,19 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>12.125</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="D51" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E51" s="1">
-        <v>0.0463</v>
+        <v>0.0454</v>
       </c>
       <c r="F51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1666,19 +1666,19 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>126.88</v>
+        <v>128.72</v>
       </c>
       <c r="C53" t="s">
         <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E53" s="1">
-        <v>0.0346</v>
+        <v>0.0355</v>
       </c>
       <c r="F53" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1689,7 +1689,7 @@
         <v>11.4</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1700,10 +1700,10 @@
         <v>2.4</v>
       </c>
       <c r="D55" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F55" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1711,16 +1711,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>16.12273</v>
+        <v>16.30909</v>
       </c>
       <c r="C56" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="E56" s="1">
-        <v>0.06519999999999999</v>
+        <v>0.066199996</v>
       </c>
       <c r="F56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1728,16 +1728,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>626.25</v>
+        <v>628.75</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E57" s="1">
-        <v>0.025</v>
+        <v>0.0252</v>
       </c>
       <c r="F57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1745,19 +1745,19 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>12.265</v>
+        <v>12.515</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D58" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E58" s="1">
-        <v>0.045700002</v>
+        <v>0.0463</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1765,19 +1765,19 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>64.68611</v>
+        <v>65.35278</v>
       </c>
       <c r="C59" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E59" s="1">
-        <v>0.031</v>
+        <v>0.0299</v>
       </c>
       <c r="F59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1785,16 +1785,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>207.4706</v>
+        <v>206</v>
       </c>
       <c r="C60" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1802,19 +1802,19 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>801.8421</v>
+        <v>802.5263</v>
       </c>
       <c r="C61" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D61" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E61" s="1">
-        <v>0.020299999</v>
+        <v>0.0202</v>
       </c>
       <c r="F61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1822,13 +1822,13 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>2.5</v>
+        <v>14.99999</v>
       </c>
       <c r="D62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1836,19 +1836,19 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>34.07368</v>
+        <v>34.23158</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="E63" s="1">
-        <v>0.0238</v>
+        <v>0.0216</v>
       </c>
       <c r="F63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1856,19 +1856,19 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>655.2057</v>
+        <v>656.50555</v>
       </c>
       <c r="C64" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D64" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E64" s="1">
-        <v>0.0055</v>
+        <v>0.0057</v>
       </c>
       <c r="F64" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1876,13 +1876,13 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>12.6125</v>
+        <v>12.66667</v>
       </c>
       <c r="D65" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="F65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1890,19 +1890,19 @@
         <v>69</v>
       </c>
       <c r="B66">
-        <v>127.454</v>
+        <v>132.7711</v>
       </c>
       <c r="C66" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D66" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E66" s="1">
-        <v>0.0323</v>
+        <v>0.031600002</v>
       </c>
       <c r="F66" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1910,16 +1910,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>15.32222</v>
+        <v>15.47647</v>
       </c>
       <c r="C67" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E67" s="1">
-        <v>0.0542</v>
+        <v>0.0538</v>
       </c>
       <c r="F67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1927,19 +1927,19 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>49.91304</v>
+        <v>50.41667</v>
       </c>
       <c r="C68" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E68" s="1">
-        <v>0.0233</v>
+        <v>0.0232</v>
       </c>
       <c r="F68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1947,19 +1947,19 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>28.7519</v>
+        <v>29.03958</v>
       </c>
       <c r="C69" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D69" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E69" s="1">
-        <v>0.0698</v>
+        <v>0.0682</v>
       </c>
       <c r="F69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1967,16 +1967,16 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>3.95385</v>
+        <v>4.16538</v>
       </c>
       <c r="C70" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1984,19 +1984,19 @@
         <v>74</v>
       </c>
       <c r="B71">
-        <v>41.41542</v>
+        <v>42.04348</v>
       </c>
       <c r="C71" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D71" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E71" s="1">
-        <v>0.0101</v>
+        <v>0.0094</v>
       </c>
       <c r="F71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2004,13 +2004,13 @@
         <v>75</v>
       </c>
       <c r="B72">
-        <v>88.50526000000001</v>
+        <v>84.00526000000001</v>
       </c>
       <c r="D72" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2018,16 +2018,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>229.61905</v>
+        <v>233.42857</v>
       </c>
       <c r="C73" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D73" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="F73" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2040,7 +2040,7 @@
         <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
26 Nov, KR,RIGL, -PFE
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="145">
   <si>
     <t>Ticker</t>
   </si>
@@ -298,7 +298,7 @@
     <t>2025-09-18</t>
   </si>
   <si>
-    <t>2025-09-10</t>
+    <t>2025-12-11</t>
   </si>
   <si>
     <t>2025-11-27</t>
@@ -328,10 +328,7 @@
     <t>2025-05-14</t>
   </si>
   <si>
-    <t>2025-03-31</t>
-  </si>
-  <si>
-    <t>2025-12-11</t>
+    <t>2025-09-30</t>
   </si>
   <si>
     <t>2024-06-14</t>
@@ -340,7 +337,7 @@
     <t>2025-04-04</t>
   </si>
   <si>
-    <t>2025-02-20</t>
+    <t>2026-02-19</t>
   </si>
   <si>
     <t>2025-11-07</t>
@@ -853,13 +850,13 @@
         <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E2" s="1">
         <v>0.0038</v>
       </c>
       <c r="F2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -873,10 +870,10 @@
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0164</v>
+        <v>0.0162</v>
       </c>
       <c r="F3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -887,7 +884,7 @@
         <v>95.26000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -895,13 +892,13 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>294.9145</v>
+        <v>294.64783</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -912,7 +909,7 @@
         <v>1.56667</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -926,10 +923,10 @@
         <v>81</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0075</v>
+        <v>0.0074</v>
       </c>
       <c r="F7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -937,19 +934,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>399.9678</v>
+        <v>401.27734</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0062</v>
+        <v>0.0061000003</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -963,13 +960,13 @@
         <v>83</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" s="1">
-        <v>0.0171</v>
+        <v>0.0168</v>
       </c>
       <c r="F9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -980,10 +977,10 @@
         <v>2.9875</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -991,7 +988,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1005,13 +1002,13 @@
         <v>84</v>
       </c>
       <c r="D12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E12" s="1">
-        <v>0.0241</v>
+        <v>0.023699999</v>
       </c>
       <c r="F12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1025,13 +1022,13 @@
         <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" s="1">
         <v>0.0215</v>
       </c>
       <c r="F13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1045,13 +1042,13 @@
         <v>86</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E14" s="1">
-        <v>0.0341</v>
+        <v>0.0339</v>
       </c>
       <c r="F14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1062,10 +1059,10 @@
         <v>3.625</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1079,13 +1076,13 @@
         <v>87</v>
       </c>
       <c r="D16" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0147</v>
+        <v>0.0145000005</v>
       </c>
       <c r="F16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1102,7 +1099,7 @@
         <v>0.0109</v>
       </c>
       <c r="F17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1113,10 +1110,10 @@
         <v>144.5</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1130,10 +1127,10 @@
         <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1147,10 +1144,10 @@
         <v>90</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0359</v>
+        <v>0.0358</v>
       </c>
       <c r="F20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1161,7 +1158,7 @@
         <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1175,13 +1172,13 @@
         <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="1">
-        <v>0.008500000000000001</v>
+        <v>0.008200000000000001</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1195,13 +1192,13 @@
         <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E23" s="1">
-        <v>0.0247</v>
+        <v>0.024300002</v>
       </c>
       <c r="F23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1215,13 +1212,13 @@
         <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0475</v>
+        <v>0.0493</v>
       </c>
       <c r="F24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1229,16 +1226,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>463.54266</v>
+        <v>463.65366</v>
       </c>
       <c r="C25" t="s">
         <v>95</v>
       </c>
       <c r="E25" s="1">
-        <v>0.024</v>
+        <v>0.0239</v>
       </c>
       <c r="F25" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1246,19 +1243,19 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>76.04545</v>
+        <v>75.95455</v>
       </c>
       <c r="C26" t="s">
         <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E26" s="1">
-        <v>0.0218</v>
+        <v>0.0212</v>
       </c>
       <c r="F26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1269,7 +1266,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1283,10 +1280,10 @@
         <v>97</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1297,10 +1294,10 @@
         <v>37.31579</v>
       </c>
       <c r="D29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1314,13 +1311,13 @@
         <v>98</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E30" s="1">
-        <v>0.0077</v>
+        <v>0.0076</v>
       </c>
       <c r="F30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1334,13 +1331,13 @@
         <v>99</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E31" s="1">
-        <v>0.0269</v>
+        <v>0.026700001</v>
       </c>
       <c r="F31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1354,13 +1351,13 @@
         <v>100</v>
       </c>
       <c r="D32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E32" s="1">
         <v>0.0116</v>
       </c>
       <c r="F32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1371,10 +1368,10 @@
         <v>134.65277</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1385,7 +1382,7 @@
         <v>19.25054</v>
       </c>
       <c r="F34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1399,13 +1396,13 @@
         <v>80</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E35" s="1">
-        <v>0.014400001</v>
+        <v>0.014199999</v>
       </c>
       <c r="F35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1416,7 +1413,7 @@
         <v>12.1</v>
       </c>
       <c r="F36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1427,10 +1424,10 @@
         <v>6.6</v>
       </c>
       <c r="D37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1441,7 +1438,7 @@
         <v>101</v>
       </c>
       <c r="F38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1452,10 +1449,10 @@
         <v>49.6</v>
       </c>
       <c r="D39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1469,10 +1466,10 @@
         <v>102</v>
       </c>
       <c r="E40" s="1">
-        <v>0.025</v>
+        <v>0.0253</v>
       </c>
       <c r="F40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1486,10 +1483,10 @@
         <v>103</v>
       </c>
       <c r="E41" s="1">
-        <v>0.0113</v>
+        <v>0.0115</v>
       </c>
       <c r="F41" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1500,13 +1497,13 @@
         <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E42" s="1">
-        <v>0.0253</v>
+        <v>0.024500001</v>
       </c>
       <c r="F42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1517,10 +1514,10 @@
         <v>13.16667</v>
       </c>
       <c r="D43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1531,10 +1528,10 @@
         <v>392.9278</v>
       </c>
       <c r="D44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1545,16 +1542,16 @@
         <v>341.90668</v>
       </c>
       <c r="C45" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E45" s="1">
         <v>0.012</v>
       </c>
       <c r="F45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1570,13 +1567,13 @@
         <v>7.2</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1584,19 +1581,19 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>399.9678</v>
+        <v>401.27734</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="D48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E48" s="1">
-        <v>0.0062</v>
+        <v>0.0061000003</v>
       </c>
       <c r="F48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1607,13 +1604,13 @@
         <v>34</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E49" s="1">
-        <v>0.0278</v>
+        <v>0.027</v>
       </c>
       <c r="F49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1624,16 +1621,16 @@
         <v>62.66667</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E50" s="1">
-        <v>0.050300002</v>
+        <v>0.0504</v>
       </c>
       <c r="F50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1647,13 +1644,13 @@
         <v>80</v>
       </c>
       <c r="D51" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E51" s="1">
-        <v>0.0454</v>
+        <v>0.045500003</v>
       </c>
       <c r="F51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1672,13 +1669,13 @@
         <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E53" s="1">
-        <v>0.0355</v>
+        <v>0.036</v>
       </c>
       <c r="F53" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1689,7 +1686,7 @@
         <v>11.4</v>
       </c>
       <c r="F54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1700,10 +1697,10 @@
         <v>2.4</v>
       </c>
       <c r="D55" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1717,10 +1714,10 @@
         <v>80</v>
       </c>
       <c r="E56" s="1">
-        <v>0.066199996</v>
+        <v>0.066300005</v>
       </c>
       <c r="F56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1728,16 +1725,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>628.75</v>
+        <v>630.25</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E57" s="1">
-        <v>0.0252</v>
+        <v>0.0279</v>
       </c>
       <c r="F57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1748,16 +1745,16 @@
         <v>12.515</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D58" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E58" s="1">
-        <v>0.0463</v>
+        <v>0.0456</v>
       </c>
       <c r="F58" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1768,16 +1765,16 @@
         <v>65.35278</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E59" s="1">
-        <v>0.0299</v>
+        <v>0.0292</v>
       </c>
       <c r="F59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1788,13 +1785,13 @@
         <v>206</v>
       </c>
       <c r="C60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F60" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1805,16 +1802,16 @@
         <v>802.5263</v>
       </c>
       <c r="C61" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E61" s="1">
-        <v>0.0202</v>
+        <v>0.0199</v>
       </c>
       <c r="F61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1825,10 +1822,10 @@
         <v>14.99999</v>
       </c>
       <c r="D62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F62" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1839,16 +1836,16 @@
         <v>34.23158</v>
       </c>
       <c r="C63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E63" s="1">
-        <v>0.0216</v>
+        <v>0.021</v>
       </c>
       <c r="F63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1859,16 +1856,16 @@
         <v>656.50555</v>
       </c>
       <c r="C64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E64" s="1">
-        <v>0.0057</v>
+        <v>0.0056</v>
       </c>
       <c r="F64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1879,10 +1876,10 @@
         <v>12.66667</v>
       </c>
       <c r="D65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1893,16 +1890,16 @@
         <v>132.7711</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E66" s="1">
-        <v>0.031600002</v>
+        <v>0.0307</v>
       </c>
       <c r="F66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1913,13 +1910,13 @@
         <v>15.47647</v>
       </c>
       <c r="C67" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E67" s="1">
-        <v>0.0538</v>
+        <v>0.053600002</v>
       </c>
       <c r="F67" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1930,16 +1927,16 @@
         <v>50.41667</v>
       </c>
       <c r="C68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E68" s="1">
         <v>0.0232</v>
       </c>
       <c r="F68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1950,16 +1947,16 @@
         <v>29.03958</v>
       </c>
       <c r="C69" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E69" s="1">
-        <v>0.0682</v>
+        <v>0.0669</v>
       </c>
       <c r="F69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1970,13 +1967,13 @@
         <v>4.16538</v>
       </c>
       <c r="C70" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1987,16 +1984,16 @@
         <v>42.04348</v>
       </c>
       <c r="C71" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D71" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E71" s="1">
-        <v>0.0094</v>
+        <v>0.0095</v>
       </c>
       <c r="F71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2007,10 +2004,10 @@
         <v>84.00526000000001</v>
       </c>
       <c r="D72" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F72" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2021,13 +2018,13 @@
         <v>233.42857</v>
       </c>
       <c r="C73" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F73" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2040,7 +2037,7 @@
         <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FIFO and Enries/Reg  formulas added in ws Entries
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="125">
   <si>
     <t>Ticker</t>
   </si>
@@ -262,7 +262,7 @@
     <t>2025-10-28</t>
   </si>
   <si>
-    <t>2025-09-22</t>
+    <t>2025-12-22</t>
   </si>
   <si>
     <t>2025-08-08</t>
@@ -277,7 +277,7 @@
     <t>2025-10-23</t>
   </si>
   <si>
-    <t>2025-12-15</t>
+    <t>2026-06-30</t>
   </si>
   <si>
     <t>2025-05-26</t>
@@ -289,9 +289,6 @@
     <t>2025-05-16</t>
   </si>
   <si>
-    <t>2025-08-25</t>
-  </si>
-  <si>
     <t>2025-12-05</t>
   </si>
   <si>
@@ -331,6 +328,9 @@
     <t>2025-09-30</t>
   </si>
   <si>
+    <t>2026-03-17</t>
+  </si>
+  <si>
     <t>2024-06-14</t>
   </si>
   <si>
@@ -352,7 +352,7 @@
     <t>2025-12-26</t>
   </si>
   <si>
-    <t>2025-10-09</t>
+    <t>2026-01-09</t>
   </si>
   <si>
     <t>2025-03-12</t>
@@ -361,6 +361,9 @@
     <t>2025-12-10</t>
   </si>
   <si>
+    <t>2026-01-23</t>
+  </si>
+  <si>
     <t>2015-08-21</t>
   </si>
   <si>
@@ -370,73 +373,10 @@
     <t>2000-03-13</t>
   </si>
   <si>
-    <t>Jan 29, 2026</t>
-  </si>
-  <si>
-    <t>Feb 5, 2026</t>
-  </si>
-  <si>
-    <t>Dec 11, 2025</t>
-  </si>
-  <si>
-    <t>Nov 6, 2025</t>
-  </si>
-  <si>
-    <t>Nov 13, 2025</t>
-  </si>
-  <si>
-    <t>Jan 14, 2026</t>
-  </si>
-  <si>
-    <t>Feb 11, 2026</t>
-  </si>
-  <si>
-    <t>Oct 29, 2025</t>
-  </si>
-  <si>
-    <t>Nov 4, 2025</t>
+    <t>--</t>
   </si>
   <si>
     <t>Oct 30, 2025</t>
-  </si>
-  <si>
-    <t>Jan 27, 2026</t>
-  </si>
-  <si>
-    <t>Dec 4, 2025</t>
-  </si>
-  <si>
-    <t>Nov 25, 2025</t>
-  </si>
-  <si>
-    <t>Jan 28, 2026</t>
-  </si>
-  <si>
-    <t>Jan 23, 2026</t>
-  </si>
-  <si>
-    <t>Oct 23, 2025</t>
-  </si>
-  <si>
-    <t>Jan 20, 2026</t>
-  </si>
-  <si>
-    <t>Nov 12, 2025</t>
-  </si>
-  <si>
-    <t>--</t>
-  </si>
-  <si>
-    <t>Jan 15, 2026</t>
-  </si>
-  <si>
-    <t>Jan 30, 2026</t>
-  </si>
-  <si>
-    <t>Oct 28, 2025</t>
-  </si>
-  <si>
-    <t>Nov 10, 2025</t>
   </si>
   <si>
     <t>USD</t>
@@ -844,19 +784,16 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>283.57733</v>
+        <v>287.70682</v>
       </c>
       <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
-        <v>118</v>
-      </c>
       <c r="E2" s="1">
-        <v>0.0037</v>
+        <v>0.0038</v>
       </c>
       <c r="F2" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -870,10 +807,10 @@
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>0.016</v>
+        <v>0.0154</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -884,7 +821,7 @@
         <v>95.26000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -892,13 +829,10 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>295.03168</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
+        <v>295.59784</v>
       </c>
       <c r="F5" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -909,7 +843,7 @@
         <v>1.56667</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -917,16 +851,16 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>983.4194</v>
+        <v>1007.8667</v>
       </c>
       <c r="C7" t="s">
         <v>81</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0067000003</v>
+        <v>0.0072000003</v>
       </c>
       <c r="F7" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -934,19 +868,16 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>409.27734</v>
+        <v>453.893</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
-      <c r="D8" t="s">
-        <v>120</v>
-      </c>
       <c r="E8" s="1">
-        <v>0.006</v>
+        <v>0.007900001</v>
       </c>
       <c r="F8" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -954,19 +885,16 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>96.86454999999999</v>
+        <v>98.95545</v>
       </c>
       <c r="C9" t="s">
         <v>83</v>
       </c>
-      <c r="D9" t="s">
-        <v>121</v>
-      </c>
       <c r="E9" s="1">
-        <v>0.0174</v>
+        <v>0.0173</v>
       </c>
       <c r="F9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -976,11 +904,8 @@
       <c r="B10">
         <v>2.9875</v>
       </c>
-      <c r="D10" t="s">
-        <v>122</v>
-      </c>
       <c r="F10" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -988,7 +913,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -996,19 +921,16 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>114.28571</v>
+        <v>118.14286</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
       </c>
-      <c r="D12" t="s">
-        <v>123</v>
-      </c>
       <c r="E12" s="1">
-        <v>0.022</v>
+        <v>0.021300001</v>
       </c>
       <c r="F12" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1016,19 +938,16 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>84.81476000000001</v>
+        <v>85.43380999999999</v>
       </c>
       <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="D13" t="s">
-        <v>124</v>
-      </c>
       <c r="E13" s="1">
-        <v>0.021</v>
+        <v>0.021300001</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1036,19 +955,16 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>91.84</v>
+        <v>94.33333</v>
       </c>
       <c r="C14" t="s">
         <v>86</v>
       </c>
-      <c r="D14" t="s">
-        <v>125</v>
-      </c>
       <c r="E14" s="1">
-        <v>0.0352</v>
+        <v>0.0342</v>
       </c>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1058,11 +974,8 @@
       <c r="B15">
         <v>3.625</v>
       </c>
-      <c r="D15" t="s">
-        <v>126</v>
-      </c>
       <c r="F15" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1075,14 +988,11 @@
       <c r="C16" t="s">
         <v>87</v>
       </c>
-      <c r="D16" t="s">
-        <v>122</v>
-      </c>
       <c r="E16" s="1">
-        <v>0.014199999</v>
+        <v>0.0134000005</v>
       </c>
       <c r="F16" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1090,16 +1000,16 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>31.65556</v>
+        <v>31.01667</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
       </c>
       <c r="E17" s="1">
-        <v>0.0109</v>
+        <v>0.011</v>
       </c>
       <c r="F17" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1109,11 +1019,8 @@
       <c r="B18">
         <v>144.5</v>
       </c>
-      <c r="D18" t="s">
-        <v>125</v>
-      </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1126,11 +1033,8 @@
       <c r="C19" t="s">
         <v>89</v>
       </c>
-      <c r="D19" t="s">
-        <v>127</v>
-      </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1138,7 +1042,7 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>16.93418</v>
+        <v>17.01653</v>
       </c>
       <c r="C20" t="s">
         <v>90</v>
@@ -1147,38 +1051,29 @@
         <v>0.0357</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="C21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22">
-        <v>74.26922999999999</v>
+        <v>79.45833</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" t="s">
-        <v>128</v>
+        <v>91</v>
       </c>
       <c r="E22" s="1">
-        <v>0.007900001</v>
+        <v>0.0074</v>
       </c>
       <c r="F22" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1186,19 +1081,16 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>26.38889</v>
+        <v>26.27778</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="E23" s="1">
-        <v>0.024400001</v>
+        <v>0.0238</v>
       </c>
       <c r="F23" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1209,16 +1101,13 @@
         <v>25.88125</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0463</v>
+        <v>0.0512</v>
       </c>
       <c r="F24" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1226,16 +1115,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>461.56952</v>
+        <v>477.35696</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E25" s="1">
-        <v>0.0242</v>
+        <v>0.0222</v>
       </c>
       <c r="F25" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1243,19 +1132,16 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>74.36364</v>
+        <v>73.52381</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="E26" s="1">
         <v>0.0223</v>
       </c>
       <c r="F26" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1266,7 +1152,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1277,13 +1163,10 @@
         <v>7.233</v>
       </c>
       <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1291,13 +1174,10 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>35.77778</v>
-      </c>
-      <c r="D29" t="s">
-        <v>121</v>
+        <v>36.75</v>
       </c>
       <c r="F29" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1305,19 +1185,16 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>625.4096</v>
+        <v>624.4480600000001</v>
       </c>
       <c r="C30" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="E30" s="1">
         <v>0.0075</v>
       </c>
       <c r="F30" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1325,19 +1202,16 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>91</v>
+        <v>91.04761999999999</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1">
-        <v>0.0273</v>
+        <v>0.027999999</v>
       </c>
       <c r="F31" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1345,19 +1219,16 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>104.779</v>
+        <v>108.895</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
-      </c>
-      <c r="D32" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0111</v>
+        <v>0.0101</v>
       </c>
       <c r="F32" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1365,13 +1236,10 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>133.41245</v>
-      </c>
-      <c r="D33" t="s">
-        <v>134</v>
+        <v>126.19184</v>
       </c>
       <c r="F33" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1382,7 +1250,7 @@
         <v>19.25054</v>
       </c>
       <c r="F34" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1390,19 +1258,16 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>47.75</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
         <v>80</v>
       </c>
-      <c r="D35" t="s">
-        <v>135</v>
-      </c>
       <c r="E35" s="1">
-        <v>0.0126</v>
+        <v>0.0112</v>
       </c>
       <c r="F35" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1413,7 +1278,7 @@
         <v>12.1</v>
       </c>
       <c r="F36" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1423,11 +1288,8 @@
       <c r="B37">
         <v>6.93333</v>
       </c>
-      <c r="D37" t="s">
-        <v>122</v>
-      </c>
       <c r="F37" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1435,13 +1297,13 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="F38" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1451,11 +1313,8 @@
       <c r="B39">
         <v>49.6</v>
       </c>
-      <c r="D39" t="s">
-        <v>126</v>
-      </c>
       <c r="F39" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1463,16 +1322,16 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>48.17647</v>
+        <v>49.13889</v>
       </c>
       <c r="C40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E40" s="1">
         <v>0.0255</v>
       </c>
       <c r="F40" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1480,16 +1339,16 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>286.75</v>
+        <v>283.205</v>
       </c>
       <c r="C41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E41" s="1">
-        <v>0.011</v>
+        <v>0.0114</v>
       </c>
       <c r="F41" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1497,16 +1356,13 @@
         <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
-      </c>
-      <c r="D42" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="E42" s="1">
-        <v>0.0227</v>
+        <v>0.023</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1516,11 +1372,8 @@
       <c r="B43">
         <v>13.16667</v>
       </c>
-      <c r="D43" t="s">
-        <v>122</v>
-      </c>
       <c r="F43" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1528,13 +1381,10 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>392.9278</v>
-      </c>
-      <c r="D44" t="s">
-        <v>131</v>
+        <v>395.726</v>
       </c>
       <c r="F44" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1542,19 +1392,16 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>341.90668</v>
+        <v>344.57333</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
-      </c>
-      <c r="D45" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0114</v>
+        <v>0.0117999995</v>
       </c>
       <c r="F45" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1572,11 +1419,8 @@
       <c r="C47" t="s">
         <v>105</v>
       </c>
-      <c r="D47" t="s">
-        <v>126</v>
-      </c>
       <c r="F47" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1584,19 +1428,16 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>409.27734</v>
+        <v>453.893</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
-      <c r="D48" t="s">
-        <v>120</v>
-      </c>
       <c r="E48" s="1">
-        <v>0.006</v>
+        <v>0.007900001</v>
       </c>
       <c r="F48" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1610,10 +1451,10 @@
         <v>106</v>
       </c>
       <c r="E49" s="1">
-        <v>0.0254</v>
+        <v>0.0253</v>
       </c>
       <c r="F49" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1621,19 +1462,19 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>62.66667</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
         <v>106</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="E50" s="1">
-        <v>0.049000002</v>
+        <v>0.047199998</v>
       </c>
       <c r="F50" t="s">
-        <v>144</v>
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1641,19 +1482,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>12.125</v>
+        <v>12.44444</v>
       </c>
       <c r="C51" t="s">
         <v>80</v>
       </c>
-      <c r="D51" t="s">
-        <v>121</v>
-      </c>
       <c r="E51" s="1">
-        <v>0.043899998</v>
+        <v>0.0402</v>
       </c>
       <c r="F51" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1666,19 +1504,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>128.92</v>
+        <v>131.56</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="E53" s="1">
         <v>0.0354</v>
       </c>
       <c r="F53" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1689,7 +1524,7 @@
         <v>11.4</v>
       </c>
       <c r="F54" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1699,11 +1534,8 @@
       <c r="B55">
         <v>2.4</v>
       </c>
-      <c r="D55" t="s">
-        <v>121</v>
-      </c>
       <c r="F55" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1711,16 +1543,16 @@
         <v>59</v>
       </c>
       <c r="B56">
-        <v>16.4</v>
+        <v>16.53636</v>
       </c>
       <c r="C56" t="s">
         <v>80</v>
       </c>
       <c r="E56" s="1">
-        <v>0.0646</v>
+        <v>0.06610000000000001</v>
       </c>
       <c r="F56" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1728,16 +1560,16 @@
         <v>60</v>
       </c>
       <c r="B57">
-        <v>615.75</v>
+        <v>607.6319999999999</v>
       </c>
       <c r="C57" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E57" s="1">
-        <v>0.027</v>
+        <v>0.0256</v>
       </c>
       <c r="F57" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1745,19 +1577,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>12.64</v>
+        <v>12.89316</v>
       </c>
       <c r="C58" t="s">
         <v>107</v>
       </c>
-      <c r="D58" t="s">
-        <v>133</v>
-      </c>
       <c r="E58" s="1">
-        <v>0.046</v>
+        <v>0.045</v>
       </c>
       <c r="F58" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1765,19 +1594,19 @@
         <v>62</v>
       </c>
       <c r="B59">
-        <v>66.03333000000001</v>
+        <v>68.42222</v>
       </c>
       <c r="C59" t="s">
         <v>108</v>
       </c>
       <c r="D59" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E59" s="1">
-        <v>0.0276</v>
+        <v>0.0251</v>
       </c>
       <c r="F59" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1785,16 +1614,13 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>206</v>
+        <v>206.5294</v>
       </c>
       <c r="C60" t="s">
         <v>109</v>
       </c>
-      <c r="D60" t="s">
-        <v>125</v>
-      </c>
       <c r="F60" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1802,19 +1628,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>802.5263</v>
+        <v>813.4737</v>
       </c>
       <c r="C61" t="s">
         <v>110</v>
       </c>
-      <c r="D61" t="s">
-        <v>137</v>
-      </c>
       <c r="E61" s="1">
-        <v>0.0187</v>
+        <v>0.0183</v>
       </c>
       <c r="F61" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1824,11 +1647,8 @@
       <c r="B62">
         <v>14.99999</v>
       </c>
-      <c r="D62" t="s">
-        <v>122</v>
-      </c>
       <c r="F62" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1836,19 +1656,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>34.47</v>
+        <v>37.62609</v>
       </c>
       <c r="C63" t="s">
         <v>111</v>
       </c>
-      <c r="D63" t="s">
-        <v>118</v>
-      </c>
       <c r="E63" s="1">
-        <v>0.019</v>
+        <v>0.0177</v>
       </c>
       <c r="F63" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1856,19 +1673,16 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>656.50555</v>
+        <v>657.3667</v>
       </c>
       <c r="C64" t="s">
         <v>112</v>
       </c>
-      <c r="D64" t="s">
-        <v>118</v>
-      </c>
       <c r="E64" s="1">
-        <v>0.0056</v>
+        <v>0.0061000003</v>
       </c>
       <c r="F64" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1878,11 +1692,8 @@
       <c r="B65">
         <v>12.66667</v>
       </c>
-      <c r="D65" t="s">
-        <v>121</v>
-      </c>
       <c r="F65" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1895,14 +1706,11 @@
       <c r="C66" t="s">
         <v>113</v>
       </c>
-      <c r="D66" t="s">
-        <v>139</v>
-      </c>
       <c r="E66" s="1">
-        <v>0.030199999</v>
+        <v>0.0295</v>
       </c>
       <c r="F66" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1910,16 +1718,16 @@
         <v>70</v>
       </c>
       <c r="B67">
-        <v>15.56471</v>
+        <v>15.68824</v>
       </c>
       <c r="C67" t="s">
         <v>110</v>
       </c>
       <c r="E67" s="1">
-        <v>0.0546</v>
+        <v>0.0541</v>
       </c>
       <c r="F67" t="s">
-        <v>143</v>
+        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1927,19 +1735,16 @@
         <v>71</v>
       </c>
       <c r="B68">
-        <v>50.375</v>
+        <v>49.91667</v>
       </c>
       <c r="C68" t="s">
         <v>114</v>
       </c>
-      <c r="D68" t="s">
-        <v>140</v>
-      </c>
       <c r="E68" s="1">
-        <v>0.0226</v>
+        <v>0.0242</v>
       </c>
       <c r="F68" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1947,19 +1752,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>29.03958</v>
+        <v>28.62292</v>
       </c>
       <c r="C69" t="s">
-        <v>107</v>
-      </c>
-      <c r="D69" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E69" s="1">
-        <v>0.06610000000000001</v>
+        <v>0.0687</v>
       </c>
       <c r="F69" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1967,16 +1769,13 @@
         <v>73</v>
       </c>
       <c r="B70">
-        <v>4.16538</v>
+        <v>4.15833</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
-      </c>
-      <c r="D70" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F70" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1987,16 +1786,13 @@
         <v>42.13043</v>
       </c>
       <c r="C71" t="s">
-        <v>116</v>
-      </c>
-      <c r="D71" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="E71" s="1">
-        <v>0.0091</v>
+        <v>0.0105</v>
       </c>
       <c r="F71" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2006,11 +1802,8 @@
       <c r="B72">
         <v>84.00526000000001</v>
       </c>
-      <c r="D72" t="s">
-        <v>121</v>
-      </c>
       <c r="F72" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -2018,16 +1811,13 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>234.33333</v>
+        <v>237.2381</v>
       </c>
       <c r="C73" t="s">
-        <v>117</v>
-      </c>
-      <c r="D73" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="F73" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2040,7 +1830,7 @@
         <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23/12, Macro Append Entry_A, FIFO formula in Entries
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
   <si>
     <t>Ticker</t>
   </si>
@@ -374,9 +374,6 @@
   </si>
   <si>
     <t>--</t>
-  </si>
-  <si>
-    <t>Oct 30, 2025</t>
   </si>
   <si>
     <t>USD</t>
@@ -793,7 +790,7 @@
         <v>0.0038</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -801,16 +798,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>19.75</v>
+        <v>20.5</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>0.0154</v>
+        <v>0.012</v>
       </c>
       <c r="F3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -821,7 +818,7 @@
         <v>95.26000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -832,7 +829,7 @@
         <v>295.59784</v>
       </c>
       <c r="F5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -843,7 +840,7 @@
         <v>1.56667</v>
       </c>
       <c r="F6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -857,10 +854,10 @@
         <v>81</v>
       </c>
       <c r="E7" s="1">
-        <v>0.0072000003</v>
+        <v>0.0070999996</v>
       </c>
       <c r="F7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -868,16 +865,16 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>453.893</v>
+        <v>456.79883</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="E8" s="1">
-        <v>0.007900001</v>
+        <v>0.0076</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -891,10 +888,10 @@
         <v>83</v>
       </c>
       <c r="E9" s="1">
-        <v>0.0173</v>
+        <v>0.0171</v>
       </c>
       <c r="F9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -905,7 +902,7 @@
         <v>2.9875</v>
       </c>
       <c r="F10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -913,7 +910,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -927,10 +924,10 @@
         <v>84</v>
       </c>
       <c r="E12" s="1">
-        <v>0.021300001</v>
+        <v>0.020299999</v>
       </c>
       <c r="F12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -944,10 +941,10 @@
         <v>85</v>
       </c>
       <c r="E13" s="1">
-        <v>0.021300001</v>
+        <v>0.021</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -961,10 +958,10 @@
         <v>86</v>
       </c>
       <c r="E14" s="1">
-        <v>0.0342</v>
+        <v>0.0339</v>
       </c>
       <c r="F14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -975,7 +972,7 @@
         <v>3.625</v>
       </c>
       <c r="F15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -989,10 +986,10 @@
         <v>87</v>
       </c>
       <c r="E16" s="1">
-        <v>0.0134000005</v>
+        <v>0.013300001</v>
       </c>
       <c r="F16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1009,7 +1006,7 @@
         <v>0.011</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1020,7 +1017,7 @@
         <v>144.5</v>
       </c>
       <c r="F18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1034,7 +1031,7 @@
         <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1048,10 +1045,10 @@
         <v>90</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0357</v>
+        <v>0.0349</v>
       </c>
       <c r="F20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1070,10 +1067,10 @@
         <v>91</v>
       </c>
       <c r="E22" s="1">
-        <v>0.0074</v>
+        <v>0.0072000003</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1087,10 +1084,10 @@
         <v>92</v>
       </c>
       <c r="E23" s="1">
-        <v>0.0238</v>
+        <v>0.0231</v>
       </c>
       <c r="F23" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1104,10 +1101,10 @@
         <v>93</v>
       </c>
       <c r="E24" s="1">
-        <v>0.0512</v>
+        <v>0.051799998</v>
       </c>
       <c r="F24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1115,7 +1112,7 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>477.35696</v>
+        <v>475.66858</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
@@ -1124,7 +1121,7 @@
         <v>0.0222</v>
       </c>
       <c r="F25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1138,10 +1135,10 @@
         <v>95</v>
       </c>
       <c r="E26" s="1">
-        <v>0.0223</v>
+        <v>0.0225</v>
       </c>
       <c r="F26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1152,7 +1149,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1166,7 +1163,7 @@
         <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1177,7 +1174,7 @@
         <v>36.75</v>
       </c>
       <c r="F29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1185,7 +1182,7 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>624.4480600000001</v>
+        <v>622.5141599999999</v>
       </c>
       <c r="C30" t="s">
         <v>97</v>
@@ -1194,7 +1191,7 @@
         <v>0.0075</v>
       </c>
       <c r="F30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1208,10 +1205,10 @@
         <v>98</v>
       </c>
       <c r="E31" s="1">
-        <v>0.027999999</v>
+        <v>0.028299998</v>
       </c>
       <c r="F31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1225,10 +1222,10 @@
         <v>99</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0101</v>
+        <v>0.0095</v>
       </c>
       <c r="F32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1239,7 +1236,7 @@
         <v>126.19184</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1250,7 +1247,7 @@
         <v>19.25054</v>
       </c>
       <c r="F34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1264,10 +1261,10 @@
         <v>80</v>
       </c>
       <c r="E35" s="1">
-        <v>0.0112</v>
+        <v>0.0104</v>
       </c>
       <c r="F35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1278,7 +1275,7 @@
         <v>12.1</v>
       </c>
       <c r="F36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1289,7 +1286,7 @@
         <v>6.93333</v>
       </c>
       <c r="F37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1303,7 +1300,7 @@
         <v>119</v>
       </c>
       <c r="F38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1314,7 +1311,7 @@
         <v>49.6</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1328,10 +1325,10 @@
         <v>101</v>
       </c>
       <c r="E40" s="1">
-        <v>0.0255</v>
+        <v>0.0249</v>
       </c>
       <c r="F40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1345,10 +1342,10 @@
         <v>102</v>
       </c>
       <c r="E41" s="1">
-        <v>0.0114</v>
+        <v>0.0113</v>
       </c>
       <c r="F41" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1359,10 +1356,10 @@
         <v>103</v>
       </c>
       <c r="E42" s="1">
-        <v>0.023</v>
+        <v>0.0229</v>
       </c>
       <c r="F42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1373,7 +1370,7 @@
         <v>13.16667</v>
       </c>
       <c r="F43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1381,10 +1378,10 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>395.726</v>
+        <v>399.151</v>
       </c>
       <c r="F44" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1398,10 +1395,10 @@
         <v>104</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0117999995</v>
+        <v>0.0115</v>
       </c>
       <c r="F45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1420,7 +1417,7 @@
         <v>105</v>
       </c>
       <c r="F47" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1428,16 +1425,16 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>453.893</v>
+        <v>456.79883</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="E48" s="1">
-        <v>0.007900001</v>
+        <v>0.0076</v>
       </c>
       <c r="F48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1454,7 +1451,7 @@
         <v>0.0253</v>
       </c>
       <c r="F49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1471,10 +1468,10 @@
         <v>119</v>
       </c>
       <c r="E50" s="1">
-        <v>0.047199998</v>
+        <v>0.0467</v>
       </c>
       <c r="F50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1488,10 +1485,10 @@
         <v>80</v>
       </c>
       <c r="E51" s="1">
-        <v>0.0402</v>
+        <v>0.04</v>
       </c>
       <c r="F51" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1510,10 +1507,10 @@
         <v>95</v>
       </c>
       <c r="E53" s="1">
-        <v>0.0354</v>
+        <v>0.0349</v>
       </c>
       <c r="F53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1524,7 +1521,7 @@
         <v>11.4</v>
       </c>
       <c r="F54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1535,7 +1532,7 @@
         <v>2.4</v>
       </c>
       <c r="F55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1549,10 +1546,10 @@
         <v>80</v>
       </c>
       <c r="E56" s="1">
-        <v>0.06610000000000001</v>
+        <v>0.0648</v>
       </c>
       <c r="F56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1566,10 +1563,10 @@
         <v>97</v>
       </c>
       <c r="E57" s="1">
-        <v>0.0256</v>
+        <v>0.0257</v>
       </c>
       <c r="F57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1577,16 +1574,16 @@
         <v>61</v>
       </c>
       <c r="B58">
-        <v>12.89316</v>
+        <v>12.99842</v>
       </c>
       <c r="C58" t="s">
         <v>107</v>
       </c>
       <c r="E58" s="1">
-        <v>0.045</v>
+        <v>0.0446</v>
       </c>
       <c r="F58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1599,14 +1596,11 @@
       <c r="C59" t="s">
         <v>108</v>
       </c>
-      <c r="D59" t="s">
-        <v>120</v>
-      </c>
       <c r="E59" s="1">
         <v>0.0251</v>
       </c>
       <c r="F59" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1620,7 +1614,7 @@
         <v>109</v>
       </c>
       <c r="F60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1634,10 +1628,10 @@
         <v>110</v>
       </c>
       <c r="E61" s="1">
-        <v>0.0183</v>
+        <v>0.0178</v>
       </c>
       <c r="F61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1648,7 +1642,7 @@
         <v>14.99999</v>
       </c>
       <c r="F62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1656,16 +1650,16 @@
         <v>66</v>
       </c>
       <c r="B63">
-        <v>37.62609</v>
+        <v>37.93043</v>
       </c>
       <c r="C63" t="s">
         <v>111</v>
       </c>
       <c r="E63" s="1">
-        <v>0.0177</v>
+        <v>0.017</v>
       </c>
       <c r="F63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1679,10 +1673,10 @@
         <v>112</v>
       </c>
       <c r="E64" s="1">
-        <v>0.0061000003</v>
+        <v>0.006</v>
       </c>
       <c r="F64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1690,10 +1684,10 @@
         <v>68</v>
       </c>
       <c r="B65">
-        <v>12.66667</v>
+        <v>12.77778</v>
       </c>
       <c r="F65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1707,10 +1701,10 @@
         <v>113</v>
       </c>
       <c r="E66" s="1">
-        <v>0.0295</v>
+        <v>0.0292</v>
       </c>
       <c r="F66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1724,10 +1718,10 @@
         <v>110</v>
       </c>
       <c r="E67" s="1">
-        <v>0.0541</v>
+        <v>0.0539</v>
       </c>
       <c r="F67" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1741,10 +1735,10 @@
         <v>114</v>
       </c>
       <c r="E68" s="1">
-        <v>0.0242</v>
+        <v>0.0238</v>
       </c>
       <c r="F68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1758,10 +1752,10 @@
         <v>115</v>
       </c>
       <c r="E69" s="1">
-        <v>0.0687</v>
+        <v>0.0682</v>
       </c>
       <c r="F69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1775,7 +1769,7 @@
         <v>116</v>
       </c>
       <c r="F70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1789,10 +1783,10 @@
         <v>117</v>
       </c>
       <c r="E71" s="1">
-        <v>0.0105</v>
+        <v>0.010299999</v>
       </c>
       <c r="F71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1803,7 +1797,7 @@
         <v>84.00526000000001</v>
       </c>
       <c r="F72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1817,7 +1811,7 @@
         <v>118</v>
       </c>
       <c r="F73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1830,7 +1824,7 @@
         <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trapper repeared, arch 30/12/25
</commit_message>
<xml_diff>
--- a/YahooDataOutput.xlsx
+++ b/YahooDataOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="123">
   <si>
     <t>Ticker</t>
   </si>
@@ -211,7 +211,7 @@
     <t>GS</t>
   </si>
   <si>
-    <t>LAZR</t>
+    <t>LAZRQ</t>
   </si>
   <si>
     <t>LUV</t>
@@ -371,9 +371,6 @@
   </si>
   <si>
     <t>2000-03-13</t>
-  </si>
-  <si>
-    <t>--</t>
   </si>
   <si>
     <t>USD</t>
@@ -790,7 +787,7 @@
         <v>0.0038</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -798,16 +795,16 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>20.5</v>
+        <v>22.75</v>
       </c>
       <c r="C3" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="1">
-        <v>0.012</v>
+        <v>0.0116</v>
       </c>
       <c r="F3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -818,7 +815,7 @@
         <v>95.26000000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -829,7 +826,7 @@
         <v>295.59784</v>
       </c>
       <c r="F5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -840,7 +837,7 @@
         <v>1.56667</v>
       </c>
       <c r="F6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -857,7 +854,7 @@
         <v>0.0070999996</v>
       </c>
       <c r="F7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -865,16 +862,16 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>456.79883</v>
+        <v>456.802</v>
       </c>
       <c r="C8" t="s">
         <v>82</v>
       </c>
       <c r="E8" s="1">
-        <v>0.0076</v>
+        <v>0.0074</v>
       </c>
       <c r="F8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -888,10 +885,10 @@
         <v>83</v>
       </c>
       <c r="E9" s="1">
-        <v>0.0171</v>
+        <v>0.016900001</v>
       </c>
       <c r="F9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -902,7 +899,7 @@
         <v>2.9875</v>
       </c>
       <c r="F10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -910,7 +907,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -918,7 +915,7 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>118.14286</v>
+        <v>118.61905</v>
       </c>
       <c r="C12" t="s">
         <v>84</v>
@@ -927,7 +924,7 @@
         <v>0.020299999</v>
       </c>
       <c r="F12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -941,10 +938,10 @@
         <v>85</v>
       </c>
       <c r="E13" s="1">
-        <v>0.021</v>
+        <v>0.0211</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -952,16 +949,16 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>94.33333</v>
+        <v>94.59999999999999</v>
       </c>
       <c r="C14" t="s">
         <v>86</v>
       </c>
       <c r="E14" s="1">
-        <v>0.0339</v>
+        <v>0.0332</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -972,7 +969,7 @@
         <v>3.625</v>
       </c>
       <c r="F15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -986,10 +983,10 @@
         <v>87</v>
       </c>
       <c r="E16" s="1">
-        <v>0.013300001</v>
+        <v>0.013099999</v>
       </c>
       <c r="F16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1006,7 +1003,7 @@
         <v>0.011</v>
       </c>
       <c r="F17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1017,7 +1014,7 @@
         <v>144.5</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1031,7 +1028,7 @@
         <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1045,10 +1042,10 @@
         <v>90</v>
       </c>
       <c r="E20" s="1">
-        <v>0.0349</v>
+        <v>0.0343</v>
       </c>
       <c r="F20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1070,7 +1067,7 @@
         <v>0.0072000003</v>
       </c>
       <c r="F22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1084,10 +1081,10 @@
         <v>92</v>
       </c>
       <c r="E23" s="1">
-        <v>0.0231</v>
+        <v>0.0234</v>
       </c>
       <c r="F23" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1101,10 +1098,10 @@
         <v>93</v>
       </c>
       <c r="E24" s="1">
-        <v>0.051799998</v>
+        <v>0.052800003</v>
       </c>
       <c r="F24" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1112,16 +1109,16 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>475.66858</v>
+        <v>475.4725</v>
       </c>
       <c r="C25" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="1">
-        <v>0.0222</v>
+        <v>0.0226</v>
       </c>
       <c r="F25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1129,16 +1126,16 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>73.52381</v>
+        <v>73.81818</v>
       </c>
       <c r="C26" t="s">
         <v>95</v>
       </c>
       <c r="E26" s="1">
-        <v>0.0225</v>
+        <v>0.0223</v>
       </c>
       <c r="F26" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1149,7 +1146,7 @@
         <v>15</v>
       </c>
       <c r="F27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1163,7 +1160,7 @@
         <v>96</v>
       </c>
       <c r="F28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1174,7 +1171,7 @@
         <v>36.75</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1191,7 +1188,7 @@
         <v>0.0075</v>
       </c>
       <c r="F30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1199,16 +1196,16 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>91.04761999999999</v>
+        <v>90.69091</v>
       </c>
       <c r="C31" t="s">
         <v>98</v>
       </c>
       <c r="E31" s="1">
-        <v>0.028299998</v>
+        <v>0.028199999</v>
       </c>
       <c r="F31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1216,16 +1213,16 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>108.895</v>
+        <v>109.495</v>
       </c>
       <c r="C32" t="s">
         <v>99</v>
       </c>
       <c r="E32" s="1">
-        <v>0.0095</v>
+        <v>0.01</v>
       </c>
       <c r="F32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1236,7 +1233,7 @@
         <v>126.19184</v>
       </c>
       <c r="F33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1247,7 +1244,7 @@
         <v>19.25054</v>
       </c>
       <c r="F34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1261,10 +1258,10 @@
         <v>80</v>
       </c>
       <c r="E35" s="1">
-        <v>0.0104</v>
+        <v>0.0107</v>
       </c>
       <c r="F35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1275,7 +1272,7 @@
         <v>12.1</v>
       </c>
       <c r="F36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1286,7 +1283,7 @@
         <v>6.93333</v>
       </c>
       <c r="F37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1296,11 +1293,8 @@
       <c r="C38" t="s">
         <v>100</v>
       </c>
-      <c r="D38" t="s">
-        <v>119</v>
-      </c>
       <c r="F38" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1308,10 +1302,10 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>49.6</v>
+        <v>51.2</v>
       </c>
       <c r="F39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1325,10 +1319,10 @@
         <v>101</v>
       </c>
       <c r="E40" s="1">
-        <v>0.0249</v>
+        <v>0.024400001</v>
       </c>
       <c r="F40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1345,7 +1339,7 @@
         <v>0.0113</v>
       </c>
       <c r="F41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1356,10 +1350,10 @@
         <v>103</v>
       </c>
       <c r="E42" s="1">
-        <v>0.0229</v>
+        <v>0.0226</v>
       </c>
       <c r="F42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1370,7 +1364,7 @@
         <v>13.16667</v>
       </c>
       <c r="F43" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1381,7 +1375,7 @@
         <v>399.151</v>
       </c>
       <c r="F44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1395,10 +1389,10 @@
         <v>104</v>
       </c>
       <c r="E45" s="1">
-        <v>0.0115</v>
+        <v>0.0112</v>
       </c>
       <c r="F45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1417,7 +1411,7 @@
         <v>105</v>
       </c>
       <c r="F47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1425,16 +1419,16 @@
         <v>12</v>
       </c>
       <c r="B48">
-        <v>456.79883</v>
+        <v>456.802</v>
       </c>
       <c r="C48" t="s">
         <v>82</v>
       </c>
       <c r="E48" s="1">
-        <v>0.0076</v>
+        <v>0.0074</v>
       </c>
       <c r="F48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1448,10 +1442,10 @@
         <v>106</v>
       </c>
       <c r="E49" s="1">
-        <v>0.0253</v>
+        <v>0.025</v>
       </c>
       <c r="F49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1464,14 +1458,11 @@
       <c r="C50" t="s">
         <v>106</v>
       </c>
-      <c r="D50" t="s">
-        <v>119</v>
-      </c>
       <c r="E50" s="1">
-        <v>0.0467</v>
+        <v>0.0468</v>
       </c>
       <c r="F50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1485,10 +1476,10 @@
         <v>80</v>
       </c>
       <c r="E51" s="1">
-        <v>0.04</v>
+        <v>0.0388</v>
       </c>
       <c r="F51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1507,10 +1498,10 @@
         <v>95</v>
       </c>
       <c r="E53" s="1">
-        <v>0.0349</v>
+        <v>0.0342</v>
       </c>
       <c r="F53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1521,7 +1512,7 @@
         <v>11.4</v>
       </c>
       <c r="F54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1532,7 +1523,7 @@
         <v>2.4</v>
       </c>
       <c r="F55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1546,10 +1537,10 @@
         <v>80</v>
       </c>
       <c r="E56" s="1">
-        <v>0.0648</v>
+        <v>0.06510000000000001</v>
       </c>
       <c r="F56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1563,10 +1554,10 @@
         <v>97</v>
       </c>
       <c r="E57" s="1">
-        <v>0.0257</v>
+        <v>0.026099999</v>
       </c>
       <c r="F57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1580,10 +1571,10 @@
         <v>107</v>
       </c>
       <c r="E58" s="1">
-        <v>0.0446</v>
+        <v>0.0452</v>
       </c>
       <c r="F58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1597,10 +1588,10 @@
         <v>108</v>
       </c>
       <c r="E59" s="1">
-        <v>0.0251</v>
+        <v>0.025</v>
       </c>
       <c r="F59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1614,7 +1605,7 @@
         <v>109</v>
       </c>
       <c r="F60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1628,10 +1619,10 @@
         <v>110</v>
       </c>
       <c r="E61" s="1">
-        <v>0.0178</v>
+        <v>0.0179</v>
       </c>
       <c r="F61" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1639,10 +1630,10 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>14.99999</v>
+        <v>1</v>
       </c>
       <c r="F62" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1656,10 +1647,10 @@
         <v>111</v>
       </c>
       <c r="E63" s="1">
-        <v>0.017</v>
+        <v>0.0175</v>
       </c>
       <c r="F63" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1667,7 +1658,7 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>657.3667</v>
+        <v>657.92224</v>
       </c>
       <c r="C64" t="s">
         <v>112</v>
@@ -1676,7 +1667,7 @@
         <v>0.006</v>
       </c>
       <c r="F64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1687,7 +1678,7 @@
         <v>12.77778</v>
       </c>
       <c r="F65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1701,10 +1692,10 @@
         <v>113</v>
       </c>
       <c r="E66" s="1">
-        <v>0.0292</v>
+        <v>0.0287</v>
       </c>
       <c r="F66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1718,10 +1709,10 @@
         <v>110</v>
       </c>
       <c r="E67" s="1">
-        <v>0.0539</v>
+        <v>0.0531</v>
       </c>
       <c r="F67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1738,7 +1729,7 @@
         <v>0.0238</v>
       </c>
       <c r="F68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1752,10 +1743,10 @@
         <v>115</v>
       </c>
       <c r="E69" s="1">
-        <v>0.0682</v>
+        <v>0.0688</v>
       </c>
       <c r="F69" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1769,7 +1760,7 @@
         <v>116</v>
       </c>
       <c r="F70" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1783,10 +1774,10 @@
         <v>117</v>
       </c>
       <c r="E71" s="1">
-        <v>0.010299999</v>
+        <v>0.01</v>
       </c>
       <c r="F71" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1797,7 +1788,7 @@
         <v>84.00526000000001</v>
       </c>
       <c r="F72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1811,7 +1802,7 @@
         <v>118</v>
       </c>
       <c r="F73" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1824,7 +1815,7 @@
         <v>78</v>
       </c>
       <c r="F75" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>